<commit_message>
added script for add MCC and MCG script
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="575">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1748,6 +1748,12 @@
   </si>
   <si>
     <t>Loan Processing Fee [44]</t>
+  </si>
+  <si>
+    <t>MccCode</t>
+  </si>
+  <si>
+    <t>Accounting, Auditing, and Bookkeeping Services [8931]</t>
   </si>
 </sst>
 </file>
@@ -9172,10 +9178,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF12"/>
+  <dimension ref="A1:BG12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BD1" sqref="BD1:BF12"/>
+      <selection activeCell="BG1" sqref="BG1:BG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9235,9 +9241,10 @@
     <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -9412,8 +9419,11 @@
       <c r="BF1" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="2" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG1" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -9582,8 +9592,11 @@
       <c r="BF2" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG2" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>545</v>
       </c>
@@ -9750,8 +9763,11 @@
       <c r="BF3" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG3" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>547</v>
       </c>
@@ -9918,8 +9934,11 @@
       <c r="BF4" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG4" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>549</v>
       </c>
@@ -10088,8 +10107,11 @@
       <c r="BF5" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG5" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>552</v>
       </c>
@@ -10258,8 +10280,11 @@
       <c r="BF6" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG6" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>554</v>
       </c>
@@ -10428,8 +10453,11 @@
       <c r="BF7" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG7" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>556</v>
       </c>
@@ -10598,8 +10626,11 @@
       <c r="BF8" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:58" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG8" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>558</v>
       </c>
@@ -10766,8 +10797,11 @@
       <c r="BF9" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:58" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG9" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>560</v>
       </c>
@@ -10934,8 +10968,11 @@
       <c r="BF10" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:58" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BG10" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>562</v>
       </c>
@@ -11104,8 +11141,11 @@
       <c r="BF11" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="BG11" s="9" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="BD12" s="9" t="s">
         <v>571</v>
       </c>
@@ -11114,6 +11154,9 @@
       </c>
       <c r="BF12" s="9" t="s">
         <v>40</v>
+      </c>
+      <c r="BG12" s="9" t="s">
+        <v>574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auth ECOMM - Test data changes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="594">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1808,6 +1808,9 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>RSA [001]</t>
   </si>
 </sst>
 </file>
@@ -9225,8 +9228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BY1" workbookViewId="0">
-      <selection activeCell="CH19" sqref="CH19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9639,7 +9642,7 @@
         <v>540</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>230</v>
@@ -9890,7 +9893,7 @@
         <v>540</v>
       </c>
       <c r="W3" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>230</v>
@@ -10139,7 +10142,7 @@
         <v>540</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>230</v>
@@ -10388,7 +10391,7 @@
         <v>540</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>230</v>
@@ -10639,7 +10642,7 @@
         <v>540</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>230</v>
@@ -10890,7 +10893,7 @@
         <v>540</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X7" s="9" t="s">
         <v>230</v>
@@ -11141,7 +11144,7 @@
         <v>540</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X8" s="9" t="s">
         <v>230</v>
@@ -11392,7 +11395,7 @@
         <v>540</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X9" s="9" t="s">
         <v>230</v>
@@ -11641,7 +11644,7 @@
         <v>540</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X10" s="9" t="s">
         <v>230</v>
@@ -11890,7 +11893,7 @@
         <v>540</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X11" s="9" t="s">
         <v>230</v>
@@ -12141,7 +12144,7 @@
         <v>540</v>
       </c>
       <c r="W12" s="9" t="s">
-        <v>230</v>
+        <v>593</v>
       </c>
       <c r="X12" s="9" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
added script for loan plan screen
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="585">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1778,6 +1778,12 @@
   </si>
   <si>
     <t>Holiday [H]</t>
+  </si>
+  <si>
+    <t>ProgramWalletPromotion</t>
+  </si>
+  <si>
+    <t>Program [0]</t>
   </si>
 </sst>
 </file>
@@ -9203,10 +9209,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL11"/>
+  <dimension ref="A1:BM11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BJ3" sqref="BJ3"/>
+      <selection activeCell="BG6" sqref="BG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9269,9 +9275,10 @@
     <col min="59" max="59" width="46" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -9464,8 +9471,11 @@
       <c r="BL1" s="1" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="2" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM1" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -9652,8 +9662,11 @@
       <c r="BL2" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="3" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM2" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>545</v>
       </c>
@@ -9838,8 +9851,11 @@
       <c r="BL3" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM3" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>547</v>
       </c>
@@ -10024,8 +10040,11 @@
       <c r="BL4" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="5" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM4" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>549</v>
       </c>
@@ -10212,8 +10231,11 @@
       <c r="BL5" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM5" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>552</v>
       </c>
@@ -10400,8 +10422,11 @@
       <c r="BL6" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="7" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM6" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>554</v>
       </c>
@@ -10588,8 +10613,11 @@
       <c r="BL7" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM7" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>556</v>
       </c>
@@ -10776,8 +10804,11 @@
       <c r="BL8" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="9" spans="1:64" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM8" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>558</v>
       </c>
@@ -10962,8 +10993,11 @@
       <c r="BL9" s="51" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="10" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM9" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>560</v>
       </c>
@@ -11148,8 +11182,11 @@
       <c r="BL10" s="47" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="11" spans="1:64" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM10" s="47" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>562</v>
       </c>
@@ -11335,6 +11372,9 @@
       </c>
       <c r="BL11" s="51" t="s">
         <v>230</v>
+      </c>
+      <c r="BM11" s="47" t="s">
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes as per Vishwas's and Saikat's comments
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3343" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="627">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1808,9 +1808,6 @@
     <t>RSA [001]</t>
   </si>
   <si>
-    <t>UPLOAD_PATH_CER</t>
-  </si>
-  <si>
     <t>HighRiskCountry</t>
   </si>
   <si>
@@ -1838,9 +1835,6 @@
     <t>ALLISS</t>
   </si>
   <si>
-    <t>/home/dc-user/integrated/elt_bo/data/CURR_EXCHANGE_UPLOAD</t>
-  </si>
-  <si>
     <t>ChecksumSupport</t>
   </si>
   <si>
@@ -1881,9 +1875,6 @@
   </si>
   <si>
     <t>PRINST</t>
-  </si>
-  <si>
-    <t>Adaptive Authentication</t>
   </si>
   <si>
     <t>HolidayType</t>
@@ -3077,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CY18"/>
+  <dimension ref="A1:CX18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3149,14 +3140,13 @@
     <col min="88" max="88" width="9.44140625" style="24" customWidth="1"/>
     <col min="89" max="89" width="14.44140625" style="24" customWidth="1"/>
     <col min="90" max="90" width="10.21875" style="24" customWidth="1"/>
-    <col min="91" max="91" width="17.6640625" style="24" customWidth="1"/>
-    <col min="92" max="92" width="16.109375" style="24" customWidth="1"/>
-    <col min="93" max="93" width="17.6640625" style="24" customWidth="1"/>
-    <col min="95" max="95" width="11.6640625" customWidth="1"/>
-    <col min="96" max="103" width="17.6640625" style="24" customWidth="1"/>
+    <col min="91" max="91" width="16.109375" style="24" customWidth="1"/>
+    <col min="92" max="92" width="17.6640625" style="24" customWidth="1"/>
+    <col min="94" max="94" width="11.6640625" customWidth="1"/>
+    <col min="95" max="102" width="17.6640625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:102" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -3224,7 +3214,7 @@
         <v>217</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>617</v>
+        <v>531</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>532</v>
@@ -3428,46 +3418,43 @@
         <v>590</v>
       </c>
       <c r="CM1" s="23" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="CN1" s="23" t="s">
         <v>603</v>
       </c>
-      <c r="CO1" s="23" t="s">
+      <c r="CO1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="CP1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="CQ1" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="CR1" s="23" t="s">
         <v>605</v>
       </c>
-      <c r="CP1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="CQ1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="CR1" s="23" t="s">
+      <c r="CS1" s="23" t="s">
         <v>606</v>
       </c>
-      <c r="CS1" s="23" t="s">
+      <c r="CT1" s="23" t="s">
         <v>607</v>
       </c>
-      <c r="CT1" s="23" t="s">
+      <c r="CU1" s="23" t="s">
         <v>608</v>
       </c>
-      <c r="CU1" s="23" t="s">
+      <c r="CV1" s="23" t="s">
         <v>609</v>
       </c>
-      <c r="CV1" s="23" t="s">
+      <c r="CW1" s="23" t="s">
         <v>610</v>
       </c>
-      <c r="CW1" s="23" t="s">
+      <c r="CX1" s="23" t="s">
         <v>611</v>
       </c>
-      <c r="CX1" s="23" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY1" s="23" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="2" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -3481,7 +3468,7 @@
         <v>400</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>539</v>
@@ -3720,43 +3707,40 @@
         <v>602</v>
       </c>
       <c r="CN2" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO2" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP2" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ2" s="9" t="s">
+      <c r="CP2" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ2" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR2" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS2" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT2" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU2" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV2" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW2" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX2" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX2" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY2" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="3" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>545</v>
       </c>
@@ -4007,43 +3991,40 @@
         <v>602</v>
       </c>
       <c r="CN3" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO3" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP3" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO3" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ3" s="9" t="s">
+      <c r="CP3" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ3" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR3" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS3" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT3" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU3" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV3" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW3" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX3" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX3" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY3" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="4" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>547</v>
       </c>
@@ -4294,43 +4275,40 @@
         <v>602</v>
       </c>
       <c r="CN4" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO4" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP4" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO4" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ4" s="9" t="s">
+      <c r="CP4" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ4" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR4" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS4" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT4" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU4" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV4" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW4" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX4" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX4" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY4" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="5" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>549</v>
       </c>
@@ -4583,43 +4561,40 @@
         <v>602</v>
       </c>
       <c r="CN5" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO5" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP5" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO5" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ5" s="9" t="s">
+      <c r="CP5" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ5" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR5" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS5" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT5" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU5" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV5" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW5" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX5" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX5" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY5" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>552</v>
       </c>
@@ -4872,43 +4847,40 @@
         <v>602</v>
       </c>
       <c r="CN6" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO6" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP6" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO6" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ6" s="9" t="s">
+      <c r="CP6" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ6" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR6" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS6" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT6" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU6" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV6" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW6" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX6" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX6" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY6" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="7" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>554</v>
       </c>
@@ -5161,43 +5133,40 @@
         <v>602</v>
       </c>
       <c r="CN7" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO7" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP7" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO7" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ7" s="9" t="s">
+      <c r="CP7" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ7" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR7" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS7" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT7" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU7" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV7" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW7" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX7" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX7" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY7" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="8" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>555</v>
       </c>
@@ -5450,43 +5419,40 @@
         <v>602</v>
       </c>
       <c r="CN8" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO8" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP8" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO8" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ8" s="9" t="s">
+      <c r="CP8" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ8" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR8" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS8" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT8" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU8" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV8" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW8" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX8" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX8" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY8" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="9" spans="1:103" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:102" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>556</v>
       </c>
@@ -5737,43 +5703,40 @@
         <v>602</v>
       </c>
       <c r="CN9" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO9" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP9" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO9" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ9" s="9" t="s">
+      <c r="CP9" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ9" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR9" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS9" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT9" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU9" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV9" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW9" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX9" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX9" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY9" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="10" spans="1:103" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:102" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>558</v>
       </c>
@@ -6024,43 +5987,40 @@
         <v>602</v>
       </c>
       <c r="CN10" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO10" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP10" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO10" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ10" s="9" t="s">
+      <c r="CP10" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ10" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR10" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS10" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT10" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU10" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV10" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW10" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX10" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX10" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY10" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="11" spans="1:103" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:102" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>560</v>
       </c>
@@ -6313,43 +6273,40 @@
         <v>602</v>
       </c>
       <c r="CN11" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO11" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP11" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO11" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ11" s="9" t="s">
+      <c r="CP11" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ11" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR11" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS11" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT11" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU11" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV11" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW11" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX11" s="25" t="s">
         <v>611</v>
       </c>
-      <c r="CX11" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY11" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="12" spans="1:103" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:102" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>563</v>
       </c>
@@ -6610,40 +6567,37 @@
         <v>602</v>
       </c>
       <c r="CN12" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CO12" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="CP12" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="CO12" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="CQ12" s="9" t="s">
+      <c r="CP12" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="CQ12" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="CR12" s="25" t="s">
-        <v>17</v>
+        <v>612</v>
       </c>
       <c r="CS12" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CT12" s="25" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="CU12" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="CV12" s="25" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="CW12" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="CX12" s="25" t="s">
         <v>611</v>
-      </c>
-      <c r="CX12" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="CY12" s="25" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="18" spans="79:79" x14ac:dyDescent="0.3">
@@ -8417,8 +8371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13199,37 +13153,37 @@
         <v>537</v>
       </c>
       <c r="BD1" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="BG1" s="1" t="s">
-        <v>596</v>
-      </c>
       <c r="BH1" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="BK1" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="2" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -13237,7 +13191,7 @@
         <v>538</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C2" s="47" t="s">
         <v>539</v>
@@ -13393,22 +13347,22 @@
       </c>
       <c r="BC2" s="47"/>
       <c r="BD2" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE2" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE2" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG2" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH2" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI2" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ2" s="9" t="s">
         <v>230</v>
@@ -13420,7 +13374,7 @@
         <v>230</v>
       </c>
       <c r="BM2" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN2" s="47" t="s">
         <v>230</v>
@@ -13585,23 +13539,23 @@
       <c r="BB3" s="47"/>
       <c r="BC3" s="47"/>
       <c r="BD3" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE3" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE3" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG3" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH3" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="BI3" s="9" t="s">
         <v>626</v>
       </c>
-      <c r="BI3" s="9" t="s">
-        <v>629</v>
-      </c>
       <c r="BJ3" s="9" t="s">
         <v>230</v>
       </c>
@@ -13612,7 +13566,7 @@
         <v>230</v>
       </c>
       <c r="BM3" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN3" s="47" t="s">
         <v>230</v>
@@ -13777,22 +13731,22 @@
       <c r="BB4" s="47"/>
       <c r="BC4" s="47"/>
       <c r="BD4" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE4" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE4" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF4" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG4" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH4" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI4" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ4" s="9" t="s">
         <v>230</v>
@@ -13804,7 +13758,7 @@
         <v>230</v>
       </c>
       <c r="BM4" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN4" s="47" t="s">
         <v>230</v>
@@ -13971,22 +13925,22 @@
       </c>
       <c r="BC5" s="47"/>
       <c r="BD5" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE5" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE5" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF5" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG5" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH5" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI5" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ5" s="9" t="s">
         <v>230</v>
@@ -13998,7 +13952,7 @@
         <v>230</v>
       </c>
       <c r="BM5" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN5" s="47" t="s">
         <v>230</v>
@@ -14165,22 +14119,22 @@
       </c>
       <c r="BC6" s="47"/>
       <c r="BD6" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE6" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE6" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF6" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG6" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH6" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI6" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ6" s="9" t="s">
         <v>230</v>
@@ -14192,7 +14146,7 @@
         <v>230</v>
       </c>
       <c r="BM6" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN6" s="47" t="s">
         <v>230</v>
@@ -14203,7 +14157,7 @@
         <v>554</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>230</v>
@@ -14359,22 +14313,22 @@
       </c>
       <c r="BC7" s="47"/>
       <c r="BD7" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE7" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE7" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF7" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG7" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH7" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI7" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ7" s="9" t="s">
         <v>230</v>
@@ -14386,7 +14340,7 @@
         <v>230</v>
       </c>
       <c r="BM7" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN7" s="47" t="s">
         <v>230</v>
@@ -14397,7 +14351,7 @@
         <v>555</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>230</v>
@@ -14553,22 +14507,22 @@
       </c>
       <c r="BC8" s="47"/>
       <c r="BD8" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE8" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE8" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG8" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH8" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI8" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ8" s="9" t="s">
         <v>230</v>
@@ -14580,7 +14534,7 @@
         <v>230</v>
       </c>
       <c r="BM8" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN8" s="47" t="s">
         <v>230</v>
@@ -14745,22 +14699,22 @@
       <c r="BB9" s="47"/>
       <c r="BC9" s="47"/>
       <c r="BD9" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE9" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE9" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG9" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH9" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI9" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ9" s="9" t="s">
         <v>230</v>
@@ -14772,7 +14726,7 @@
         <v>230</v>
       </c>
       <c r="BM9" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN9" s="47" t="s">
         <v>230</v>
@@ -14937,22 +14891,22 @@
       <c r="BB10" s="47"/>
       <c r="BC10" s="47"/>
       <c r="BD10" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE10" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE10" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF10" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG10" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH10" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI10" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ10" s="9" t="s">
         <v>230</v>
@@ -14964,7 +14918,7 @@
         <v>230</v>
       </c>
       <c r="BM10" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN10" s="47" t="s">
         <v>230</v>
@@ -15131,22 +15085,22 @@
       </c>
       <c r="BC11" s="47"/>
       <c r="BD11" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="BE11" s="9" t="s">
         <v>597</v>
-      </c>
-      <c r="BE11" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="BF11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BG11" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="BH11" s="9" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="BI11" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="BJ11" s="9" t="s">
         <v>230</v>
@@ -15158,7 +15112,7 @@
         <v>230</v>
       </c>
       <c r="BM11" s="47" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="BN11" s="47" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
Resolved the test data conflicts
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="LoyaltyPlan" sheetId="16" r:id="rId16"/>
     <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="674">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1911,6 +1911,147 @@
   </si>
   <si>
     <t>Retail Transaction to Loan [LOANPUR]</t>
+  </si>
+  <si>
+    <t>Padding</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>AmexInstitutionSetup</t>
+  </si>
+  <si>
+    <t>Swap</t>
+  </si>
+  <si>
+    <t>BLACKEYEFD [576771]</t>
+  </si>
+  <si>
+    <t>EMBF6000</t>
+  </si>
+  <si>
+    <t>VEN6000</t>
+  </si>
+  <si>
+    <t>HDFCVendor01 [VEN6000]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yerwada Pune </t>
+  </si>
+  <si>
+    <t>June/1/2033</t>
+  </si>
+  <si>
+    <t>235689</t>
+  </si>
+  <si>
+    <t>Amex Credit</t>
+  </si>
+  <si>
+    <t>Sequence number</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Program Code</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>IBM Method [3]</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>1234567890123456</t>
+  </si>
+  <si>
+    <t>181CFD03C3F7385FCA36BF63DDD4BD01</t>
+  </si>
+  <si>
+    <t>829DD2</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1-Single Component [1]</t>
+  </si>
+  <si>
+    <t>4A43436017024880</t>
+  </si>
+  <si>
+    <t>0EBBE7</t>
+  </si>
+  <si>
+    <t>B4638CBCEC1E6E52</t>
+  </si>
+  <si>
+    <t>985BDD</t>
+  </si>
+  <si>
+    <t>7B634E89DB88BBD9BB33C702FD1C9151</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>MasterCard(CIS) [03]</t>
+  </si>
+  <si>
+    <t>ZMK [6]</t>
+  </si>
+  <si>
+    <t>80F5706D510BF6F7D54D6DA3053CAB8A</t>
+  </si>
+  <si>
+    <t>2A7944</t>
+  </si>
+  <si>
+    <t>E60699F5B9ADE145FF6B0281D6FF7A71</t>
+  </si>
+  <si>
+    <t>2BC1FE</t>
+  </si>
+  <si>
+    <t>3B84D3C46E096114BF1A505A548A88AE</t>
+  </si>
+  <si>
+    <t>55AF3C</t>
+  </si>
+  <si>
+    <t>6B9D441DA33CF04F687C085A0CD9D8F8</t>
+  </si>
+  <si>
+    <t>9855B6</t>
+  </si>
+  <si>
+    <t>MDK Key [00]</t>
+  </si>
+  <si>
+    <t>Active [0]</t>
+  </si>
+  <si>
+    <t>InstitutionCode</t>
+  </si>
+  <si>
+    <t>Abbrevation</t>
+  </si>
+  <si>
+    <t>555522</t>
+  </si>
+  <si>
+    <t>AUTHREG</t>
   </si>
 </sst>
 </file>
@@ -2085,7 +2226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2183,6 +2324,8 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3070,8 +3213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9177,10 +9320,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DN177"/>
+  <dimension ref="A1:EP177"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9198,7 +9341,7 @@
     <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:146" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9552,7 +9695,7 @@
       </c>
       <c r="DN1" s="4"/>
     </row>
-    <row r="2" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -9879,7 +10022,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>140</v>
       </c>
@@ -10158,7 +10301,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:118" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:146" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>150</v>
       </c>
@@ -10437,7 +10580,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
@@ -10716,7 +10859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>163</v>
       </c>
@@ -10995,7 +11138,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>169</v>
       </c>
@@ -11276,7 +11419,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>175</v>
       </c>
@@ -11557,16 +11700,421 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.3">
-      <c r="CS9"/>
-      <c r="CT9" t="s">
-        <v>162</v>
-      </c>
-      <c r="CU9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>562</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R9" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="S9" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="T9" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="U9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="V9" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="W9" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="X9" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y9" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z9" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC9" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF9" s="28" t="s">
+        <v>633</v>
+      </c>
+      <c r="AG9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI9" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="AJ9" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK9" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL9" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM9" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="AN9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO9" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP9" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="AQ9" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="AR9" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="AS9" s="28" t="s">
+        <v>634</v>
+      </c>
+      <c r="AT9" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU9" s="28" t="s">
+        <v>635</v>
+      </c>
+      <c r="AV9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW9" s="29"/>
+      <c r="AX9" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="AY9" s="28" t="s">
+        <v>636</v>
+      </c>
+      <c r="AZ9" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB9" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="BC9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD9" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="BE9" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF9" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="BG9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH9" s="28"/>
+      <c r="BI9" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="BJ9" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="BK9" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="BL9" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM9" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="BN9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="BO9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="BP9" s="28" t="s">
+        <v>409</v>
+      </c>
+      <c r="BQ9" s="28"/>
+      <c r="BR9" s="2"/>
+      <c r="BS9" s="9"/>
+      <c r="BT9" s="9"/>
+      <c r="BU9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BV9" s="9"/>
+      <c r="BW9" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="BX9" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="BY9" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="CA9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="CB9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="CC9" s="28" t="s">
+        <v>637</v>
+      </c>
+      <c r="CD9" s="9"/>
+      <c r="CE9" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="CF9" s="28"/>
+      <c r="CG9" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="CH9" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="CI9" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="CJ9" s="28" t="s">
+        <v>412</v>
+      </c>
+      <c r="CK9" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="CL9" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="CM9" s="28"/>
+      <c r="CN9" s="28"/>
+      <c r="CO9" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP9" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="CQ9" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="CR9" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="CS9" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="CT9" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="CU9" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="CV9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="CW9" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="CX9" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="CY9" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="CZ9" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="DA9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="DB9" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="DC9" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="DD9" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="DE9" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="DF9" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="DG9" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="DH9" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="DI9" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="DJ9" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="DK9" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="DL9" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="DM9" s="50" t="s">
+        <v>645</v>
+      </c>
+      <c r="DN9" s="50" t="s">
+        <v>494</v>
+      </c>
+      <c r="DO9" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="DP9" s="55" t="s">
+        <v>647</v>
+      </c>
+      <c r="DQ9" s="55" t="s">
+        <v>648</v>
+      </c>
+      <c r="DR9" s="55" t="s">
+        <v>649</v>
+      </c>
+      <c r="DS9" s="55" t="s">
+        <v>650</v>
+      </c>
+      <c r="DT9" s="55" t="s">
+        <v>651</v>
+      </c>
+      <c r="DU9" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="DV9" s="55" t="s">
+        <v>653</v>
+      </c>
+      <c r="DW9" s="55" t="s">
+        <v>654</v>
+      </c>
+      <c r="DX9" s="55" t="s">
+        <v>655</v>
+      </c>
+      <c r="DY9" s="55" t="s">
+        <v>656</v>
+      </c>
+      <c r="DZ9" s="55" t="s">
+        <v>657</v>
+      </c>
+      <c r="EA9" s="55" t="s">
+        <v>406</v>
+      </c>
+      <c r="EB9" s="55" t="s">
+        <v>406</v>
+      </c>
+      <c r="EC9" s="55" t="s">
+        <v>406</v>
+      </c>
+      <c r="ED9" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="EE9" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="EF9" s="50" t="s">
+        <v>660</v>
+      </c>
+      <c r="EG9" s="50" t="s">
+        <v>661</v>
+      </c>
+      <c r="EH9" s="50" t="s">
+        <v>662</v>
+      </c>
+      <c r="EI9" s="50" t="s">
+        <v>663</v>
+      </c>
+      <c r="EJ9" s="50" t="s">
+        <v>664</v>
+      </c>
+      <c r="EK9" s="50" t="s">
+        <v>665</v>
+      </c>
+      <c r="EL9" s="50" t="s">
+        <v>666</v>
+      </c>
+      <c r="EM9" s="50" t="s">
+        <v>667</v>
+      </c>
+      <c r="EN9" s="56" t="s">
+        <v>668</v>
+      </c>
+      <c r="EO9" s="56" t="s">
+        <v>505</v>
+      </c>
+      <c r="EP9" s="56" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS10"/>
       <c r="CT10" t="s">
         <v>162</v>
@@ -11575,7 +12123,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS11"/>
       <c r="CT11" t="s">
         <v>162</v>
@@ -11584,19 +12132,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS12"/>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CS16"/>
     </row>
     <row r="17" spans="97:97" x14ac:dyDescent="0.3">
@@ -12916,488 +13464,498 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN11"/>
+  <dimension ref="A1:BQ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="34" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="24" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="46" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="24" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="15" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="46" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="F1" s="45" t="s">
         <v>295</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="G1" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="H1" s="45" t="s">
         <v>297</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="I1" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="J1" s="45" t="s">
         <v>299</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="K1" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="L1" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="M1" s="45" t="s">
         <v>357</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="N1" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="O1" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="P1" s="45" t="s">
         <v>358</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="Q1" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="R1" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="S1" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="T1" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="R1" s="45" t="s">
+      <c r="U1" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="V1" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="W1" s="45" t="s">
         <v>531</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="X1" s="45" t="s">
         <v>532</v>
       </c>
-      <c r="V1" s="45" t="s">
+      <c r="Y1" s="45" t="s">
         <v>533</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="Z1" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="X1" s="45" t="s">
+      <c r="AA1" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="AB1" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="AC1" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="AA1" s="45" t="s">
+      <c r="AD1" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="AB1" s="45" t="s">
+      <c r="AE1" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="AC1" s="45" t="s">
+      <c r="AF1" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="AD1" s="45" t="s">
+      <c r="AG1" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="AE1" s="45" t="s">
+      <c r="AH1" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="AF1" s="45" t="s">
+      <c r="AI1" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="AG1" s="45" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>359</v>
       </c>
-      <c r="AH1" s="45" t="s">
+      <c r="AK1" s="45" t="s">
         <v>360</v>
       </c>
-      <c r="AI1" s="45" t="s">
+      <c r="AL1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="AJ1" s="45" t="s">
+      <c r="AM1" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="AK1" s="45" t="s">
+      <c r="AN1" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="AL1" s="45" t="s">
+      <c r="AO1" s="45" t="s">
         <v>361</v>
       </c>
-      <c r="AM1" s="45" t="s">
+      <c r="AP1" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="AN1" s="45" t="s">
+      <c r="AQ1" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="AO1" s="45" t="s">
+      <c r="AR1" s="45" t="s">
         <v>364</v>
       </c>
-      <c r="AP1" s="45" t="s">
+      <c r="AS1" s="45" t="s">
         <v>365</v>
       </c>
-      <c r="AQ1" s="45" t="s">
+      <c r="AT1" s="45" t="s">
         <v>366</v>
       </c>
-      <c r="AR1" s="45" t="s">
+      <c r="AU1" s="45" t="s">
         <v>367</v>
       </c>
-      <c r="AS1" s="45" t="s">
+      <c r="AV1" s="45" t="s">
         <v>368</v>
       </c>
-      <c r="AT1" s="45" t="s">
+      <c r="AW1" s="45" t="s">
         <v>369</v>
       </c>
-      <c r="AU1" s="45" t="s">
+      <c r="AX1" s="45" t="s">
         <v>370</v>
       </c>
-      <c r="AV1" s="45" t="s">
+      <c r="AY1" s="45" t="s">
         <v>371</v>
       </c>
-      <c r="AW1" s="45" t="s">
+      <c r="AZ1" s="45" t="s">
         <v>372</v>
       </c>
-      <c r="AX1" s="45" t="s">
+      <c r="BA1" s="45" t="s">
         <v>373</v>
       </c>
-      <c r="AY1" s="45" t="s">
+      <c r="BB1" s="45" t="s">
         <v>374</v>
       </c>
-      <c r="AZ1" s="45" t="s">
+      <c r="BC1" s="45" t="s">
         <v>534</v>
       </c>
-      <c r="BA1" s="45" t="s">
+      <c r="BD1" s="45" t="s">
         <v>535</v>
       </c>
-      <c r="BB1" s="45" t="s">
+      <c r="BE1" s="45" t="s">
         <v>536</v>
       </c>
-      <c r="BC1" s="45" t="s">
+      <c r="BF1" s="45" t="s">
         <v>537</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="2" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>622</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="G2" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="E2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="51" t="s">
+      <c r="H2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="H2" s="47" t="s">
+      <c r="J2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="K2" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="I2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2" s="47" t="s">
+      <c r="L2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M2" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M2" s="47" t="s">
+      <c r="N2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P2" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="47" t="s">
+      <c r="Q2" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O2" s="51" t="s">
+      <c r="R2" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q2" s="47">
+      <c r="S2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T2" s="47">
         <v>16</v>
       </c>
-      <c r="R2" s="47">
+      <c r="U2" s="47">
         <v>16</v>
       </c>
-      <c r="S2" s="47" t="s">
+      <c r="V2" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T2" s="47" t="s">
+      <c r="W2" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W2" s="47">
+      <c r="X2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z2" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X2" s="47" t="s">
+      <c r="AA2" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y2" s="47">
+      <c r="AB2" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z2" s="47" t="s">
+      <c r="AC2" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA2" s="47" t="s">
+      <c r="AD2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="47">
+      <c r="AE2" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC2" s="47">
+      <c r="AF2" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD2" s="52" t="s">
+      <c r="AG2" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE2" s="47" t="s">
+      <c r="AH2" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF2" s="47" t="s">
+      <c r="AI2" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG2" s="47" t="s">
+      <c r="AJ2" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH2" s="47" t="s">
+      <c r="AK2" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI2" s="47" t="s">
+      <c r="AL2" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="47" t="s">
+      <c r="AM2" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK2" s="47">
+      <c r="AN2" s="47">
         <v>411006</v>
       </c>
-      <c r="AL2" s="47">
+      <c r="AO2" s="47">
         <v>124421</v>
       </c>
-      <c r="AM2" s="47" t="s">
+      <c r="AP2" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN2" s="47" t="s">
+      <c r="AQ2" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO2" s="47" t="s">
+      <c r="AR2" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP2" s="47" t="s">
+      <c r="AS2" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ2" s="47"/>
-      <c r="AR2" s="47"/>
-      <c r="AS2" s="47" t="s">
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT2" s="47" t="s">
+      <c r="AW2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU2" s="47">
+      <c r="AX2" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV2" s="47" t="s">
+      <c r="AY2" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW2" s="47" t="s">
+      <c r="AZ2" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX2" s="47">
+      <c r="BA2" s="47">
         <v>999</v>
       </c>
-      <c r="AY2" s="47" t="s">
+      <c r="BB2" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ2" s="47" t="s">
+      <c r="BC2" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA2" s="47" t="s">
+      <c r="BD2" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB2" s="47" t="s">
+      <c r="BE2" s="47" t="s">
         <v>544</v>
       </c>
-      <c r="BC2" s="47"/>
-      <c r="BD2" s="9" t="s">
+      <c r="BF2" s="47"/>
+      <c r="BG2" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE2" s="9" t="s">
+      <c r="BH2" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF2" s="9" t="s">
+      <c r="BI2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG2" s="9" t="s">
+      <c r="BJ2" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH2" s="9" t="s">
+      <c r="BK2" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI2" s="9" t="s">
+      <c r="BL2" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL2" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM2" s="47" t="s">
+      <c r="BM2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP2" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN2" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ2" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>545</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>546</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="F3" s="51" t="s">
-        <v>134</v>
+      <c r="C3" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="47" t="s">
+        <v>230</v>
       </c>
       <c r="G3" s="47" t="s">
         <v>539</v>
@@ -13405,1159 +13963,1193 @@
       <c r="H3" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="I3" s="47" t="s">
-        <v>230</v>
+      <c r="I3" s="51" t="s">
+        <v>134</v>
       </c>
       <c r="J3" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="K3" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="L3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M3" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M3" s="47" t="s">
+      <c r="N3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P3" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="47" t="s">
+      <c r="Q3" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O3" s="51" t="s">
+      <c r="R3" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q3" s="47">
+      <c r="S3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T3" s="47">
         <v>16</v>
       </c>
-      <c r="R3" s="47">
+      <c r="U3" s="47">
         <v>16</v>
       </c>
-      <c r="S3" s="47" t="s">
+      <c r="V3" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T3" s="47" t="s">
+      <c r="W3" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W3" s="47">
+      <c r="X3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z3" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X3" s="47" t="s">
+      <c r="AA3" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y3" s="47">
+      <c r="AB3" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z3" s="47" t="s">
+      <c r="AC3" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA3" s="47" t="s">
+      <c r="AD3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="47">
+      <c r="AE3" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC3" s="47">
+      <c r="AF3" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD3" s="52" t="s">
+      <c r="AG3" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE3" s="47" t="s">
+      <c r="AH3" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF3" s="47" t="s">
+      <c r="AI3" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG3" s="47" t="s">
+      <c r="AJ3" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH3" s="47" t="s">
+      <c r="AK3" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI3" s="47" t="s">
+      <c r="AL3" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ3" s="47" t="s">
+      <c r="AM3" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK3" s="47">
+      <c r="AN3" s="47">
         <v>411006</v>
       </c>
-      <c r="AL3" s="47">
+      <c r="AO3" s="47">
         <v>124421</v>
       </c>
-      <c r="AM3" s="47" t="s">
+      <c r="AP3" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN3" s="47" t="s">
+      <c r="AQ3" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO3" s="47" t="s">
+      <c r="AR3" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP3" s="47" t="s">
+      <c r="AS3" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ3" s="47"/>
-      <c r="AR3" s="47"/>
-      <c r="AS3" s="47" t="s">
+      <c r="AT3" s="47"/>
+      <c r="AU3" s="47"/>
+      <c r="AV3" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT3" s="47" t="s">
+      <c r="AW3" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU3" s="47">
+      <c r="AX3" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV3" s="47" t="s">
+      <c r="AY3" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW3" s="47" t="s">
+      <c r="AZ3" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX3" s="47">
+      <c r="BA3" s="47">
         <v>999</v>
       </c>
-      <c r="AY3" s="47" t="s">
+      <c r="BB3" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ3" s="47" t="s">
+      <c r="BC3" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA3" s="47" t="s">
+      <c r="BD3" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB3" s="47"/>
-      <c r="BC3" s="47"/>
-      <c r="BD3" s="9" t="s">
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="47"/>
+      <c r="BG3" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE3" s="9" t="s">
+      <c r="BH3" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF3" s="9" t="s">
+      <c r="BI3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG3" s="9" t="s">
+      <c r="BJ3" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH3" s="9" t="s">
+      <c r="BK3" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI3" s="9" t="s">
+      <c r="BL3" s="9" t="s">
         <v>626</v>
       </c>
-      <c r="BJ3" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK3" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL3" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM3" s="47" t="s">
+      <c r="BM3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO3" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP3" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN3" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ3" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>547</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>548</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="D4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E4" s="47" t="s">
+      <c r="G4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="H4" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="I4" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="J4" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="H4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="I4" s="47" t="s">
+      <c r="K4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="M4" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M4" s="47" t="s">
+      <c r="N4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P4" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="47" t="s">
+      <c r="Q4" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O4" s="51" t="s">
+      <c r="R4" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q4" s="47">
+      <c r="S4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T4" s="47">
         <v>16</v>
       </c>
-      <c r="R4" s="47">
+      <c r="U4" s="47">
         <v>16</v>
       </c>
-      <c r="S4" s="47" t="s">
+      <c r="V4" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T4" s="47" t="s">
+      <c r="W4" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W4" s="47">
+      <c r="X4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z4" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X4" s="47" t="s">
+      <c r="AA4" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y4" s="47">
+      <c r="AB4" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z4" s="47" t="s">
+      <c r="AC4" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA4" s="47" t="s">
+      <c r="AD4" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="47">
+      <c r="AE4" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC4" s="47">
+      <c r="AF4" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD4" s="52" t="s">
+      <c r="AG4" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE4" s="47" t="s">
+      <c r="AH4" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF4" s="47" t="s">
+      <c r="AI4" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG4" s="47" t="s">
+      <c r="AJ4" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH4" s="47" t="s">
+      <c r="AK4" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI4" s="47" t="s">
+      <c r="AL4" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ4" s="47" t="s">
+      <c r="AM4" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK4" s="47">
+      <c r="AN4" s="47">
         <v>411006</v>
       </c>
-      <c r="AL4" s="47">
+      <c r="AO4" s="47">
         <v>124421</v>
       </c>
-      <c r="AM4" s="47" t="s">
+      <c r="AP4" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN4" s="47" t="s">
+      <c r="AQ4" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO4" s="47" t="s">
+      <c r="AR4" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP4" s="47" t="s">
+      <c r="AS4" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="47" t="s">
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT4" s="47" t="s">
+      <c r="AW4" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU4" s="47">
+      <c r="AX4" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV4" s="47" t="s">
+      <c r="AY4" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW4" s="47" t="s">
+      <c r="AZ4" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX4" s="47">
+      <c r="BA4" s="47">
         <v>999</v>
       </c>
-      <c r="AY4" s="47" t="s">
+      <c r="BB4" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ4" s="47" t="s">
+      <c r="BC4" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA4" s="47" t="s">
+      <c r="BD4" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB4" s="47"/>
-      <c r="BC4" s="47"/>
-      <c r="BD4" s="9" t="s">
+      <c r="BE4" s="47"/>
+      <c r="BF4" s="47"/>
+      <c r="BG4" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE4" s="9" t="s">
+      <c r="BH4" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF4" s="9" t="s">
+      <c r="BI4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG4" s="9" t="s">
+      <c r="BJ4" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH4" s="9" t="s">
+      <c r="BK4" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI4" s="9" t="s">
+      <c r="BL4" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ4" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK4" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL4" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM4" s="47" t="s">
+      <c r="BM4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO4" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP4" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN4" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ4" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>549</v>
       </c>
       <c r="B5" s="47" t="s">
         <v>550</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="D5" s="47" t="s">
+      <c r="C5" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="G5" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="E5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="F5" s="51" t="s">
+      <c r="H5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I5" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="H5" s="47" t="s">
+      <c r="J5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="K5" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="I5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="J5" s="47" t="s">
+      <c r="L5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M5" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M5" s="47" t="s">
+      <c r="N5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P5" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N5" s="47" t="s">
+      <c r="Q5" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O5" s="51" t="s">
+      <c r="R5" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q5" s="47">
+      <c r="S5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T5" s="47">
         <v>16</v>
       </c>
-      <c r="R5" s="47">
+      <c r="U5" s="47">
         <v>16</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="V5" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T5" s="47" t="s">
+      <c r="W5" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W5" s="47">
+      <c r="X5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z5" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X5" s="47" t="s">
+      <c r="AA5" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y5" s="47">
+      <c r="AB5" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z5" s="47" t="s">
+      <c r="AC5" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA5" s="47" t="s">
+      <c r="AD5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB5" s="47">
+      <c r="AE5" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC5" s="47">
+      <c r="AF5" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD5" s="52" t="s">
+      <c r="AG5" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE5" s="47" t="s">
+      <c r="AH5" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF5" s="47" t="s">
+      <c r="AI5" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG5" s="47" t="s">
+      <c r="AJ5" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH5" s="47" t="s">
+      <c r="AK5" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI5" s="47" t="s">
+      <c r="AL5" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ5" s="47" t="s">
+      <c r="AM5" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK5" s="47">
+      <c r="AN5" s="47">
         <v>411006</v>
       </c>
-      <c r="AL5" s="47">
+      <c r="AO5" s="47">
         <v>124421</v>
       </c>
-      <c r="AM5" s="47" t="s">
+      <c r="AP5" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN5" s="47" t="s">
+      <c r="AQ5" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO5" s="47" t="s">
+      <c r="AR5" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP5" s="47" t="s">
+      <c r="AS5" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ5" s="47"/>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="47" t="s">
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT5" s="47" t="s">
+      <c r="AW5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU5" s="47">
+      <c r="AX5" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV5" s="47" t="s">
+      <c r="AY5" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW5" s="47" t="s">
+      <c r="AZ5" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX5" s="47">
+      <c r="BA5" s="47">
         <v>999</v>
       </c>
-      <c r="AY5" s="47" t="s">
+      <c r="BB5" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ5" s="47" t="s">
+      <c r="BC5" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA5" s="47" t="s">
+      <c r="BD5" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB5" s="47" t="s">
+      <c r="BE5" s="47" t="s">
         <v>551</v>
       </c>
-      <c r="BC5" s="47"/>
-      <c r="BD5" s="9" t="s">
+      <c r="BF5" s="47"/>
+      <c r="BG5" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE5" s="9" t="s">
+      <c r="BH5" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF5" s="9" t="s">
+      <c r="BI5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG5" s="9" t="s">
+      <c r="BJ5" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH5" s="9" t="s">
+      <c r="BK5" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI5" s="9" t="s">
+      <c r="BL5" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ5" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK5" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL5" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM5" s="47" t="s">
+      <c r="BM5" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN5" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO5" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP5" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN5" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ5" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>552</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>553</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="D6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="F6" s="51" t="s">
+      <c r="G6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I6" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>230</v>
-      </c>
       <c r="J6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="K6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="L6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M6" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M6" s="47" t="s">
+      <c r="N6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P6" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="Q6" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="51" t="s">
+      <c r="R6" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q6" s="47">
+      <c r="S6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T6" s="47">
         <v>16</v>
       </c>
-      <c r="R6" s="47">
+      <c r="U6" s="47">
         <v>16</v>
       </c>
-      <c r="S6" s="47" t="s">
+      <c r="V6" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T6" s="47" t="s">
+      <c r="W6" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W6" s="47">
+      <c r="X6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z6" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X6" s="47" t="s">
+      <c r="AA6" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y6" s="47">
+      <c r="AB6" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z6" s="47" t="s">
+      <c r="AC6" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA6" s="47" t="s">
+      <c r="AD6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB6" s="47">
+      <c r="AE6" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC6" s="47">
+      <c r="AF6" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD6" s="52" t="s">
+      <c r="AG6" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE6" s="47" t="s">
+      <c r="AH6" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF6" s="47" t="s">
+      <c r="AI6" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG6" s="47" t="s">
+      <c r="AJ6" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH6" s="47" t="s">
+      <c r="AK6" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI6" s="47" t="s">
+      <c r="AL6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ6" s="47" t="s">
+      <c r="AM6" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK6" s="47">
+      <c r="AN6" s="47">
         <v>411006</v>
       </c>
-      <c r="AL6" s="47">
+      <c r="AO6" s="47">
         <v>124421</v>
       </c>
-      <c r="AM6" s="47" t="s">
+      <c r="AP6" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN6" s="47" t="s">
+      <c r="AQ6" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO6" s="47" t="s">
+      <c r="AR6" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP6" s="47" t="s">
+      <c r="AS6" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ6" s="47"/>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47" t="s">
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT6" s="47" t="s">
+      <c r="AW6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU6" s="47">
+      <c r="AX6" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV6" s="47" t="s">
+      <c r="AY6" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW6" s="47" t="s">
+      <c r="AZ6" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX6" s="47">
+      <c r="BA6" s="47">
         <v>999</v>
       </c>
-      <c r="AY6" s="47" t="s">
+      <c r="BB6" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ6" s="47" t="s">
+      <c r="BC6" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA6" s="47" t="s">
+      <c r="BD6" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB6" s="47" t="s">
+      <c r="BE6" s="47" t="s">
         <v>544</v>
       </c>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="9" t="s">
+      <c r="BF6" s="47"/>
+      <c r="BG6" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BH6" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BI6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG6" s="9" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH6" s="9" t="s">
+      <c r="BK6" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI6" s="9" t="s">
+      <c r="BL6" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ6" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK6" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL6" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM6" s="47" t="s">
+      <c r="BM6" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN6" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO6" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP6" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN6" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ6" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>554</v>
       </c>
       <c r="B7" s="47" t="s">
         <v>599</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E7" s="47" t="s">
+      <c r="C7" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="H7" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="I7" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="J7" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="H7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="I7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="J7" s="47" t="s">
+      <c r="K7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="L7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M7" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M7" s="47" t="s">
+      <c r="N7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P7" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="47" t="s">
+      <c r="Q7" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="51" t="s">
+      <c r="R7" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q7" s="47">
+      <c r="S7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T7" s="47">
         <v>16</v>
       </c>
-      <c r="R7" s="47">
+      <c r="U7" s="47">
         <v>16</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="V7" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="W7" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W7" s="47">
+      <c r="X7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z7" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X7" s="47" t="s">
+      <c r="AA7" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y7" s="47">
+      <c r="AB7" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z7" s="47" t="s">
+      <c r="AC7" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA7" s="47" t="s">
+      <c r="AD7" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB7" s="47">
+      <c r="AE7" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC7" s="47">
+      <c r="AF7" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD7" s="52" t="s">
+      <c r="AG7" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE7" s="47" t="s">
+      <c r="AH7" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF7" s="47" t="s">
+      <c r="AI7" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG7" s="47" t="s">
+      <c r="AJ7" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH7" s="47" t="s">
+      <c r="AK7" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI7" s="47" t="s">
+      <c r="AL7" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ7" s="47" t="s">
+      <c r="AM7" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK7" s="47">
+      <c r="AN7" s="47">
         <v>411006</v>
       </c>
-      <c r="AL7" s="47">
+      <c r="AO7" s="47">
         <v>124421</v>
       </c>
-      <c r="AM7" s="47" t="s">
+      <c r="AP7" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN7" s="47" t="s">
+      <c r="AQ7" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO7" s="47" t="s">
+      <c r="AR7" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP7" s="47" t="s">
+      <c r="AS7" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ7" s="47"/>
-      <c r="AR7" s="47"/>
-      <c r="AS7" s="47" t="s">
+      <c r="AT7" s="47"/>
+      <c r="AU7" s="47"/>
+      <c r="AV7" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT7" s="47" t="s">
+      <c r="AW7" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU7" s="47">
+      <c r="AX7" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV7" s="47" t="s">
+      <c r="AY7" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW7" s="47" t="s">
+      <c r="AZ7" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX7" s="47">
+      <c r="BA7" s="47">
         <v>999</v>
       </c>
-      <c r="AY7" s="47" t="s">
+      <c r="BB7" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ7" s="47" t="s">
+      <c r="BC7" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA7" s="47" t="s">
+      <c r="BD7" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB7" s="47" t="s">
+      <c r="BE7" s="47" t="s">
         <v>544</v>
       </c>
-      <c r="BC7" s="47"/>
-      <c r="BD7" s="9" t="s">
+      <c r="BF7" s="47"/>
+      <c r="BG7" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE7" s="9" t="s">
+      <c r="BH7" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF7" s="9" t="s">
+      <c r="BI7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG7" s="9" t="s">
+      <c r="BJ7" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH7" s="9" t="s">
+      <c r="BK7" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI7" s="9" t="s">
+      <c r="BL7" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ7" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK7" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL7" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM7" s="47" t="s">
+      <c r="BM7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO7" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP7" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN7" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ7" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>555</v>
       </c>
       <c r="B8" s="47" t="s">
         <v>600</v>
       </c>
-      <c r="C8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="51" t="s">
+      <c r="C8" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I8" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="I8" s="47" t="s">
-        <v>230</v>
-      </c>
       <c r="J8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="K8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="L8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M8" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M8" s="47" t="s">
+      <c r="N8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P8" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="47" t="s">
+      <c r="Q8" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="51" t="s">
+      <c r="R8" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q8" s="47">
+      <c r="S8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T8" s="47">
         <v>16</v>
       </c>
-      <c r="R8" s="47">
+      <c r="U8" s="47">
         <v>16</v>
       </c>
-      <c r="S8" s="47" t="s">
+      <c r="V8" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T8" s="47" t="s">
+      <c r="W8" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W8" s="47">
+      <c r="X8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z8" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X8" s="47" t="s">
+      <c r="AA8" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y8" s="47">
+      <c r="AB8" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z8" s="47" t="s">
+      <c r="AC8" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA8" s="47" t="s">
+      <c r="AD8" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB8" s="47">
+      <c r="AE8" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC8" s="47">
+      <c r="AF8" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD8" s="52" t="s">
+      <c r="AG8" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE8" s="47" t="s">
+      <c r="AH8" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF8" s="47" t="s">
+      <c r="AI8" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG8" s="47" t="s">
+      <c r="AJ8" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH8" s="47" t="s">
+      <c r="AK8" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI8" s="47" t="s">
+      <c r="AL8" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ8" s="47" t="s">
+      <c r="AM8" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK8" s="47">
+      <c r="AN8" s="47">
         <v>411006</v>
       </c>
-      <c r="AL8" s="47">
+      <c r="AO8" s="47">
         <v>124421</v>
       </c>
-      <c r="AM8" s="47" t="s">
+      <c r="AP8" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN8" s="47" t="s">
+      <c r="AQ8" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO8" s="47" t="s">
+      <c r="AR8" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP8" s="47" t="s">
+      <c r="AS8" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ8" s="47"/>
-      <c r="AR8" s="47"/>
-      <c r="AS8" s="47" t="s">
+      <c r="AT8" s="47"/>
+      <c r="AU8" s="47"/>
+      <c r="AV8" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT8" s="47" t="s">
+      <c r="AW8" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU8" s="47">
+      <c r="AX8" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV8" s="47" t="s">
+      <c r="AY8" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW8" s="47" t="s">
+      <c r="AZ8" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX8" s="47">
+      <c r="BA8" s="47">
         <v>999</v>
       </c>
-      <c r="AY8" s="47" t="s">
+      <c r="BB8" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ8" s="47" t="s">
+      <c r="BC8" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA8" s="47" t="s">
+      <c r="BD8" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB8" s="47" t="s">
+      <c r="BE8" s="47" t="s">
         <v>544</v>
       </c>
-      <c r="BC8" s="47"/>
-      <c r="BD8" s="9" t="s">
+      <c r="BF8" s="47"/>
+      <c r="BG8" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE8" s="9" t="s">
+      <c r="BH8" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF8" s="9" t="s">
+      <c r="BI8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG8" s="9" t="s">
+      <c r="BJ8" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH8" s="9" t="s">
+      <c r="BK8" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI8" s="9" t="s">
+      <c r="BL8" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ8" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK8" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL8" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM8" s="47" t="s">
+      <c r="BM8" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN8" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO8" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP8" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN8" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:66" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ8" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>556</v>
       </c>
       <c r="B9" s="47" t="s">
         <v>557</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>134</v>
+      <c r="C9" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="47" t="s">
+        <v>230</v>
       </c>
       <c r="G9" s="47" t="s">
         <v>539</v>
@@ -14565,581 +15157,605 @@
       <c r="H9" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="I9" s="47" t="s">
-        <v>230</v>
+      <c r="I9" s="51" t="s">
+        <v>134</v>
       </c>
       <c r="J9" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="K9" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="L9" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M9" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K9" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L9" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M9" s="47" t="s">
+      <c r="N9" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O9" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P9" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="47" t="s">
+      <c r="Q9" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O9" s="51" t="s">
+      <c r="R9" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P9" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q9" s="47">
+      <c r="S9" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T9" s="47">
         <v>16</v>
       </c>
-      <c r="R9" s="47">
+      <c r="U9" s="47">
         <v>16</v>
       </c>
-      <c r="S9" s="47" t="s">
+      <c r="V9" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T9" s="47" t="s">
+      <c r="W9" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U9" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V9" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W9" s="47">
+      <c r="X9" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y9" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z9" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X9" s="47" t="s">
+      <c r="AA9" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y9" s="47">
+      <c r="AB9" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z9" s="47" t="s">
+      <c r="AC9" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA9" s="47" t="s">
+      <c r="AD9" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB9" s="47">
+      <c r="AE9" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC9" s="47">
+      <c r="AF9" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD9" s="52" t="s">
+      <c r="AG9" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE9" s="47" t="s">
+      <c r="AH9" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF9" s="47" t="s">
+      <c r="AI9" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG9" s="47" t="s">
+      <c r="AJ9" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH9" s="47" t="s">
+      <c r="AK9" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI9" s="47" t="s">
+      <c r="AL9" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ9" s="47" t="s">
+      <c r="AM9" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK9" s="47">
+      <c r="AN9" s="47">
         <v>411006</v>
       </c>
-      <c r="AL9" s="47">
+      <c r="AO9" s="47">
         <v>124421</v>
       </c>
-      <c r="AM9" s="47" t="s">
+      <c r="AP9" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN9" s="47" t="s">
+      <c r="AQ9" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO9" s="47" t="s">
+      <c r="AR9" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP9" s="47" t="s">
+      <c r="AS9" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ9" s="47"/>
-      <c r="AR9" s="47"/>
-      <c r="AS9" s="47" t="s">
+      <c r="AT9" s="47"/>
+      <c r="AU9" s="47"/>
+      <c r="AV9" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT9" s="47" t="s">
+      <c r="AW9" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU9" s="47">
+      <c r="AX9" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV9" s="47" t="s">
+      <c r="AY9" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW9" s="47" t="s">
+      <c r="AZ9" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX9" s="47">
+      <c r="BA9" s="47">
         <v>999</v>
       </c>
-      <c r="AY9" s="47" t="s">
+      <c r="BB9" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ9" s="47" t="s">
+      <c r="BC9" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA9" s="47" t="s">
+      <c r="BD9" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB9" s="47"/>
-      <c r="BC9" s="47"/>
-      <c r="BD9" s="9" t="s">
+      <c r="BE9" s="47"/>
+      <c r="BF9" s="47"/>
+      <c r="BG9" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE9" s="9" t="s">
+      <c r="BH9" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF9" s="9" t="s">
+      <c r="BI9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG9" s="9" t="s">
+      <c r="BJ9" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH9" s="9" t="s">
+      <c r="BK9" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI9" s="9" t="s">
+      <c r="BL9" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ9" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK9" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL9" s="53" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM9" s="47" t="s">
+      <c r="BM9" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN9" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO9" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP9" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN9" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ9" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>558</v>
       </c>
       <c r="B10" s="47" t="s">
         <v>559</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="D10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>134</v>
-      </c>
       <c r="G10" s="47" t="s">
-        <v>539</v>
+        <v>230</v>
       </c>
       <c r="H10" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="I10" s="47" t="s">
-        <v>230</v>
+      <c r="I10" s="51" t="s">
+        <v>134</v>
       </c>
       <c r="J10" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="K10" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="L10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M10" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M10" s="47" t="s">
+      <c r="N10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P10" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="47" t="s">
+      <c r="Q10" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O10" s="51" t="s">
+      <c r="R10" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q10" s="47">
+      <c r="S10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T10" s="47">
         <v>16</v>
       </c>
-      <c r="R10" s="47">
+      <c r="U10" s="47">
         <v>16</v>
       </c>
-      <c r="S10" s="47" t="s">
+      <c r="V10" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T10" s="47" t="s">
+      <c r="W10" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W10" s="47">
+      <c r="X10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z10" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X10" s="47" t="s">
+      <c r="AA10" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y10" s="47">
+      <c r="AB10" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z10" s="47" t="s">
+      <c r="AC10" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA10" s="47" t="s">
+      <c r="AD10" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB10" s="47">
+      <c r="AE10" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC10" s="47">
+      <c r="AF10" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD10" s="52" t="s">
+      <c r="AG10" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE10" s="47" t="s">
+      <c r="AH10" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF10" s="47" t="s">
+      <c r="AI10" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG10" s="47" t="s">
+      <c r="AJ10" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH10" s="47" t="s">
+      <c r="AK10" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI10" s="47" t="s">
+      <c r="AL10" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ10" s="47" t="s">
+      <c r="AM10" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK10" s="47">
+      <c r="AN10" s="47">
         <v>411006</v>
       </c>
-      <c r="AL10" s="47">
+      <c r="AO10" s="47">
         <v>124421</v>
       </c>
-      <c r="AM10" s="47" t="s">
+      <c r="AP10" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN10" s="47" t="s">
+      <c r="AQ10" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO10" s="47" t="s">
+      <c r="AR10" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP10" s="47" t="s">
+      <c r="AS10" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ10" s="47"/>
-      <c r="AR10" s="47"/>
-      <c r="AS10" s="47" t="s">
+      <c r="AT10" s="47"/>
+      <c r="AU10" s="47"/>
+      <c r="AV10" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT10" s="47" t="s">
+      <c r="AW10" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU10" s="47">
+      <c r="AX10" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV10" s="47" t="s">
+      <c r="AY10" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW10" s="47" t="s">
+      <c r="AZ10" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX10" s="47">
+      <c r="BA10" s="47">
         <v>999</v>
       </c>
-      <c r="AY10" s="47" t="s">
+      <c r="BB10" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ10" s="47" t="s">
+      <c r="BC10" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA10" s="47" t="s">
+      <c r="BD10" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB10" s="47"/>
-      <c r="BC10" s="47"/>
-      <c r="BD10" s="9" t="s">
+      <c r="BE10" s="47"/>
+      <c r="BF10" s="47"/>
+      <c r="BG10" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE10" s="9" t="s">
+      <c r="BH10" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF10" s="9" t="s">
+      <c r="BI10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG10" s="9" t="s">
+      <c r="BJ10" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH10" s="9" t="s">
+      <c r="BK10" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI10" s="9" t="s">
+      <c r="BL10" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ10" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK10" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL10" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM10" s="47" t="s">
+      <c r="BM10" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN10" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO10" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP10" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN10" s="47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:66" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BQ10" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>560</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>561</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="F11" s="51" t="s">
+      <c r="C11" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I11" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="J11" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="H11" s="47" t="s">
+      <c r="K11" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="I11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="J11" s="47" t="s">
+      <c r="L11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="M11" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="M11" s="47" t="s">
+      <c r="N11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="O11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="P11" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="N11" s="47" t="s">
+      <c r="Q11" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="O11" s="51" t="s">
+      <c r="R11" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="P11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q11" s="47">
+      <c r="S11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="T11" s="47">
         <v>16</v>
       </c>
-      <c r="R11" s="47">
+      <c r="U11" s="47">
         <v>16</v>
       </c>
-      <c r="S11" s="47" t="s">
+      <c r="V11" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="T11" s="47" t="s">
+      <c r="W11" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="U11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="V11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="W11" s="47">
+      <c r="X11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y11" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z11" s="47">
         <v>1100440052</v>
       </c>
-      <c r="X11" s="47" t="s">
+      <c r="AA11" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="Y11" s="47">
+      <c r="AB11" s="47">
         <v>45665456</v>
       </c>
-      <c r="Z11" s="47" t="s">
+      <c r="AC11" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AA11" s="47" t="s">
+      <c r="AD11" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AB11" s="47">
+      <c r="AE11" s="47">
         <v>1113332</v>
       </c>
-      <c r="AC11" s="47">
+      <c r="AF11" s="47">
         <v>23564589</v>
       </c>
-      <c r="AD11" s="52" t="s">
+      <c r="AG11" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="AE11" s="47" t="s">
+      <c r="AH11" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AF11" s="47" t="s">
+      <c r="AI11" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AG11" s="47" t="s">
+      <c r="AJ11" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AH11" s="47" t="s">
+      <c r="AK11" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AI11" s="47" t="s">
+      <c r="AL11" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AJ11" s="47" t="s">
+      <c r="AM11" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AK11" s="47">
+      <c r="AN11" s="47">
         <v>411006</v>
       </c>
-      <c r="AL11" s="47">
+      <c r="AO11" s="47">
         <v>124421</v>
       </c>
-      <c r="AM11" s="47" t="s">
+      <c r="AP11" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="AN11" s="47" t="s">
+      <c r="AQ11" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="AO11" s="47" t="s">
+      <c r="AR11" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="AP11" s="47" t="s">
+      <c r="AS11" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="AQ11" s="47"/>
-      <c r="AR11" s="47"/>
-      <c r="AS11" s="47" t="s">
+      <c r="AT11" s="47"/>
+      <c r="AU11" s="47"/>
+      <c r="AV11" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="AT11" s="47" t="s">
+      <c r="AW11" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AU11" s="47">
+      <c r="AX11" s="47">
         <v>5431267812</v>
       </c>
-      <c r="AV11" s="47" t="s">
+      <c r="AY11" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="AW11" s="47" t="s">
+      <c r="AZ11" s="47" t="s">
         <v>379</v>
       </c>
-      <c r="AX11" s="47">
+      <c r="BA11" s="47">
         <v>999</v>
       </c>
-      <c r="AY11" s="47" t="s">
+      <c r="BB11" s="47" t="s">
         <v>380</v>
       </c>
-      <c r="AZ11" s="47" t="s">
+      <c r="BC11" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="BA11" s="47" t="s">
+      <c r="BD11" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="BB11" s="47" t="s">
+      <c r="BE11" s="47" t="s">
         <v>544</v>
       </c>
-      <c r="BC11" s="47"/>
-      <c r="BD11" s="9" t="s">
+      <c r="BF11" s="47"/>
+      <c r="BG11" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="BE11" s="9" t="s">
+      <c r="BH11" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="BF11" s="9" t="s">
+      <c r="BI11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BG11" s="9" t="s">
+      <c r="BJ11" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="BH11" s="9" t="s">
+      <c r="BK11" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="BI11" s="9" t="s">
+      <c r="BL11" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="BJ11" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK11" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL11" s="53" t="s">
-        <v>230</v>
-      </c>
-      <c r="BM11" s="47" t="s">
+      <c r="BM11" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BN11" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BO11" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="BP11" s="47" t="s">
         <v>625</v>
       </c>
-      <c r="BN11" s="47" t="s">
-        <v>230</v>
-      </c>
+      <c r="BQ11" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="X2" r:id="rId1"/>
-    <hyperlink ref="AD2" r:id="rId2"/>
-    <hyperlink ref="X3" r:id="rId3"/>
-    <hyperlink ref="AD3" r:id="rId4"/>
-    <hyperlink ref="X5" r:id="rId5"/>
-    <hyperlink ref="AD5" r:id="rId6"/>
-    <hyperlink ref="X6" r:id="rId7"/>
-    <hyperlink ref="AD6" r:id="rId8"/>
-    <hyperlink ref="X4" r:id="rId9"/>
-    <hyperlink ref="AD4" r:id="rId10"/>
-    <hyperlink ref="X7" r:id="rId11"/>
-    <hyperlink ref="AD7" r:id="rId12"/>
-    <hyperlink ref="X8" r:id="rId13"/>
-    <hyperlink ref="AD8" r:id="rId14"/>
-    <hyperlink ref="X9" r:id="rId15"/>
-    <hyperlink ref="AD9" r:id="rId16"/>
-    <hyperlink ref="X10" r:id="rId17"/>
-    <hyperlink ref="AD10" r:id="rId18"/>
-    <hyperlink ref="X11" r:id="rId19"/>
-    <hyperlink ref="AD11" r:id="rId20"/>
+    <hyperlink ref="AA2" r:id="rId1"/>
+    <hyperlink ref="AG2" r:id="rId2"/>
+    <hyperlink ref="AA3" r:id="rId3"/>
+    <hyperlink ref="AG3" r:id="rId4"/>
+    <hyperlink ref="AA5" r:id="rId5"/>
+    <hyperlink ref="AG5" r:id="rId6"/>
+    <hyperlink ref="AA6" r:id="rId7"/>
+    <hyperlink ref="AG6" r:id="rId8"/>
+    <hyperlink ref="AA4" r:id="rId9"/>
+    <hyperlink ref="AG4" r:id="rId10"/>
+    <hyperlink ref="AA7" r:id="rId11"/>
+    <hyperlink ref="AG7" r:id="rId12"/>
+    <hyperlink ref="AA8" r:id="rId13"/>
+    <hyperlink ref="AG8" r:id="rId14"/>
+    <hyperlink ref="AA9" r:id="rId15"/>
+    <hyperlink ref="AG9" r:id="rId16"/>
+    <hyperlink ref="AA10" r:id="rId17"/>
+    <hyperlink ref="AG10" r:id="rId18"/>
+    <hyperlink ref="AA11" r:id="rId19"/>
+    <hyperlink ref="AG11" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>

</xml_diff>

<commit_message>
Instituion prority setup template creation
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="CardHolder" sheetId="20" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="LoyaltyPlan" sheetId="16" r:id="rId17"/>
     <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId18"/>
     <sheet name="InstituteSetup" sheetId="18" r:id="rId19"/>
+    <sheet name="Priority_setup" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4438" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4639" uniqueCount="868">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2612,6 +2613,30 @@
   </si>
   <si>
     <t>TC_visaMoneyTransfer</t>
+  </si>
+  <si>
+    <t>Lengh12</t>
+  </si>
+  <si>
+    <t>FirstCustomValue12</t>
+  </si>
+  <si>
+    <t>SecondCustomValue12</t>
+  </si>
+  <si>
+    <t>Institution_priority_setup</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>2136547985</t>
+  </si>
+  <si>
+    <t>7776542135</t>
+  </si>
+  <si>
+    <t>BIN [1]</t>
   </si>
 </sst>
 </file>
@@ -2621,7 +2646,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2672,6 +2697,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2816,7 +2848,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2933,6 +2965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -3241,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12133,7 +12166,7 @@
   <dimension ref="A1:DA18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16372,6 +16405,686 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DF2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="107" max="107" width="26.85546875" customWidth="1"/>
+    <col min="108" max="108" width="28" customWidth="1"/>
+    <col min="109" max="110" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:110" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="BQ1" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="BR1" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="BS1" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="BT1" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="BU1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BV1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="BW1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="BX1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="BY1" s="15" t="s">
+        <v>691</v>
+      </c>
+      <c r="BZ1" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="CA1" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="CB1" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="CC1" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="CD1" s="23" t="s">
+        <v>331</v>
+      </c>
+      <c r="CE1" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="CF1" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="CG1" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="CH1" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="CI1" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="CJ1" s="23" t="s">
+        <v>341</v>
+      </c>
+      <c r="CK1" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="CL1" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="CM1" s="23" t="s">
+        <v>343</v>
+      </c>
+      <c r="CN1" s="23" t="s">
+        <v>344</v>
+      </c>
+      <c r="CO1" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="CP1" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="CQ1" s="23" t="s">
+        <v>694</v>
+      </c>
+      <c r="CR1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="CS1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="CT1" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="CU1" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="CV1" s="23" t="s">
+        <v>697</v>
+      </c>
+      <c r="CW1" s="23" t="s">
+        <v>698</v>
+      </c>
+      <c r="CX1" s="23" t="s">
+        <v>699</v>
+      </c>
+      <c r="CY1" s="23" t="s">
+        <v>700</v>
+      </c>
+      <c r="CZ1" s="23" t="s">
+        <v>701</v>
+      </c>
+      <c r="DA1" s="23" t="s">
+        <v>702</v>
+      </c>
+      <c r="DB1" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="DC1" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="DD1" s="74" t="s">
+        <v>862</v>
+      </c>
+      <c r="DE1" s="74" t="s">
+        <v>429</v>
+      </c>
+      <c r="DF1" s="74" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:110" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>863</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>864</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="W2" s="9">
+        <v>16</v>
+      </c>
+      <c r="X2" s="9">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC2" s="9">
+        <v>1100440052</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH2" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="AI2" s="9">
+        <v>23564589</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AQ2" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AR2" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="AT2" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="AU2" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA2" s="9">
+        <v>5431267812</v>
+      </c>
+      <c r="BB2" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="BC2" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="BD2" s="9">
+        <v>999</v>
+      </c>
+      <c r="BE2" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="BF2" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="BG2" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="BH2" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="BK2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BM2" s="9">
+        <v>121212</v>
+      </c>
+      <c r="BN2" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="BP2" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="BW2" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="BY2" s="2"/>
+      <c r="BZ2" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="CA2" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="CB2" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="CC2" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="CD2" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="CE2" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="CF2" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="CG2" s="25"/>
+      <c r="CH2" s="25"/>
+      <c r="CI2" s="25">
+        <v>121212</v>
+      </c>
+      <c r="CJ2" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="CK2" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="CL2" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="CM2" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="CN2" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="CO2" s="25"/>
+      <c r="CP2" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="CQ2" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="CR2" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="CS2" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="CT2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="CU2" s="25" t="s">
+        <v>713</v>
+      </c>
+      <c r="CV2" s="25" t="s">
+        <v>713</v>
+      </c>
+      <c r="CW2" s="25" t="s">
+        <v>713</v>
+      </c>
+      <c r="CX2" s="25" t="s">
+        <v>714</v>
+      </c>
+      <c r="CY2" s="25" t="s">
+        <v>700</v>
+      </c>
+      <c r="CZ2" s="25" t="s">
+        <v>701</v>
+      </c>
+      <c r="DA2" s="25" t="s">
+        <v>702</v>
+      </c>
+      <c r="DB2" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="DC2" s="9" t="s">
+        <v>865</v>
+      </c>
+      <c r="DD2" s="9" t="s">
+        <v>866</v>
+      </c>
+      <c r="DE2" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="DF2" s="9" t="s">
+        <v>589</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select from the dropdown" sqref="CM2">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AD2" r:id="rId1"/>
+    <hyperlink ref="AJ2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FD177"/>

</xml_diff>

<commit_message>
Added SHEET10 to the TestData.xlsx for StageSA, demo and Automation2
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -4,28 +4,29 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CardHolder" sheetId="20" r:id="rId1"/>
-    <sheet name="S181372" sheetId="1" r:id="rId2"/>
-    <sheet name="S205014" sheetId="2" r:id="rId3"/>
-    <sheet name="S205000" sheetId="3" r:id="rId4"/>
-    <sheet name="AuditReport" sheetId="19" r:id="rId5"/>
-    <sheet name="S205009" sheetId="6" r:id="rId6"/>
-    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId7"/>
-    <sheet name="AccounHeadMapping_S205175" sheetId="8" r:id="rId8"/>
-    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId9"/>
-    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId10"/>
-    <sheet name="Institute" sheetId="5" r:id="rId11"/>
-    <sheet name="ApplicationUpload" sheetId="11" r:id="rId12"/>
-    <sheet name="AmlockDownloads" sheetId="15" r:id="rId13"/>
-    <sheet name="CurrencyExchangeRates" sheetId="12" r:id="rId14"/>
-    <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId15"/>
-    <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId16"/>
-    <sheet name="LoyaltyPlan" sheetId="16" r:id="rId17"/>
-    <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId18"/>
-    <sheet name="InstituteSetup" sheetId="18" r:id="rId19"/>
+    <sheet name="SHEET10" sheetId="21" r:id="rId2"/>
+    <sheet name="S181372" sheetId="1" r:id="rId3"/>
+    <sheet name="S205014" sheetId="2" r:id="rId4"/>
+    <sheet name="S205000" sheetId="3" r:id="rId5"/>
+    <sheet name="AuditReport" sheetId="19" r:id="rId6"/>
+    <sheet name="S205009" sheetId="6" r:id="rId7"/>
+    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId8"/>
+    <sheet name="AccounHeadMapping_S205175" sheetId="8" r:id="rId9"/>
+    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId10"/>
+    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId11"/>
+    <sheet name="Institute" sheetId="5" r:id="rId12"/>
+    <sheet name="ApplicationUpload" sheetId="11" r:id="rId13"/>
+    <sheet name="AmlockDownloads" sheetId="15" r:id="rId14"/>
+    <sheet name="CurrencyExchangeRates" sheetId="12" r:id="rId15"/>
+    <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId16"/>
+    <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId17"/>
+    <sheet name="LoyaltyPlan" sheetId="16" r:id="rId18"/>
+    <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId19"/>
+    <sheet name="InstituteSetup" sheetId="18" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -3241,18 +3242,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>1</v>
       </c>
@@ -3422,7 +3423,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
         <v>797</v>
       </c>
@@ -3516,7 +3517,7 @@
       <c r="BC2" s="64"/>
       <c r="BD2" s="64"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>808</v>
       </c>
@@ -3590,7 +3591,7 @@
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>809</v>
       </c>
@@ -3664,7 +3665,7 @@
       <c r="BC4" s="2"/>
       <c r="BD4" s="2"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>811</v>
       </c>
@@ -3754,7 +3755,7 @@
       <c r="BC5" s="2"/>
       <c r="BD5" s="2"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>816</v>
       </c>
@@ -3828,7 +3829,7 @@
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>817</v>
       </c>
@@ -3908,7 +3909,7 @@
       <c r="BC7" s="2"/>
       <c r="BD7" s="2"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>820</v>
       </c>
@@ -3992,7 +3993,7 @@
       <c r="BC8" s="2"/>
       <c r="BD8" s="2"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>823</v>
       </c>
@@ -4084,7 +4085,7 @@
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>828</v>
       </c>
@@ -4176,7 +4177,7 @@
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>829</v>
       </c>
@@ -4274,7 +4275,7 @@
       <c r="BC11" s="2"/>
       <c r="BD11" s="2"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>832</v>
       </c>
@@ -4372,7 +4373,7 @@
       <c r="BC12" s="2"/>
       <c r="BD12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>834</v>
       </c>
@@ -4472,7 +4473,7 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>836</v>
       </c>
@@ -4572,7 +4573,7 @@
       <c r="BC14" s="2"/>
       <c r="BD14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>837</v>
       </c>
@@ -4672,7 +4673,7 @@
       <c r="BC15" s="2"/>
       <c r="BD15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>838</v>
       </c>
@@ -4776,7 +4777,7 @@
       <c r="BC16" s="2"/>
       <c r="BD16" s="2"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" s="64" t="s">
         <v>848</v>
       </c>
@@ -4884,7 +4885,7 @@
       <c r="BC17" s="64"/>
       <c r="BD17" s="64"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>849</v>
       </c>
@@ -4992,7 +4993,7 @@
       <c r="BC18" s="2"/>
       <c r="BD18" s="2"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>850</v>
       </c>
@@ -5100,7 +5101,7 @@
       <c r="BC19" s="2"/>
       <c r="BD19" s="2"/>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>851</v>
       </c>
@@ -5208,7 +5209,7 @@
       <c r="BC20" s="2"/>
       <c r="BD20" s="2"/>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>852</v>
       </c>
@@ -5282,7 +5283,7 @@
       <c r="BC21" s="2"/>
       <c r="BD21" s="2"/>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>853</v>
       </c>
@@ -5356,7 +5357,7 @@
       <c r="BC22" s="2"/>
       <c r="BD22" s="2"/>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>854</v>
       </c>
@@ -5430,7 +5431,7 @@
       <c r="BC23" s="2"/>
       <c r="BD23" s="2"/>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>855</v>
       </c>
@@ -5504,7 +5505,7 @@
       <c r="BC24" s="2"/>
       <c r="BD24" s="2"/>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>856</v>
       </c>
@@ -5578,7 +5579,7 @@
       <c r="BC25" s="2"/>
       <c r="BD25" s="2"/>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>857</v>
       </c>
@@ -5652,7 +5653,7 @@
       <c r="BC26" s="2"/>
       <c r="BD26" s="2"/>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>858</v>
       </c>
@@ -5726,7 +5727,7 @@
       <c r="BC27" s="2"/>
       <c r="BD27" s="2"/>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>859</v>
       </c>
@@ -5830,18 +5831,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5858,47 +5857,75 @@
         <v>256</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>207</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>207</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="2">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -5908,80 +5935,158 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DD12"/>
   <sheetViews>
     <sheetView topLeftCell="CH1" workbookViewId="0">
       <selection activeCell="CY5" sqref="CY5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="24" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="15" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="46" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="15" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="30" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:108" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -6307,7 +6412,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="2" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -6615,7 +6720,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="3" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>545</v>
       </c>
@@ -6921,7 +7026,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="4" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>547</v>
       </c>
@@ -7227,7 +7332,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="5" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>549</v>
       </c>
@@ -7535,7 +7640,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="6" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>552</v>
       </c>
@@ -7843,7 +7948,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>554</v>
       </c>
@@ -8151,7 +8256,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="8" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>556</v>
       </c>
@@ -8463,7 +8568,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="9" spans="1:108" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:108" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>558</v>
       </c>
@@ -8769,7 +8874,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="10" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:108" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>560</v>
       </c>
@@ -9075,7 +9180,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="11" spans="1:108" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:108" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>562</v>
       </c>
@@ -9383,7 +9488,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="12" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:108" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="9"/>
@@ -9596,7 +9701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
@@ -9604,12 +9709,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -9663,7 +9768,7 @@
       </c>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>301</v>
       </c>
@@ -9716,7 +9821,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -9769,7 +9874,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>303</v>
       </c>
@@ -9822,7 +9927,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -9875,7 +9980,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -9933,7 +10038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -9941,18 +10046,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="33" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="31"/>
+    <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9972,7 +10077,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>382</v>
       </c>
@@ -9992,7 +10097,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>383</v>
       </c>
@@ -10012,7 +10117,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>390</v>
       </c>
@@ -10032,7 +10137,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>384</v>
       </c>
@@ -10052,7 +10157,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>385</v>
       </c>
@@ -10072,7 +10177,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>386</v>
       </c>
@@ -10092,7 +10197,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>387</v>
       </c>
@@ -10117,7 +10222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -10125,27 +10230,27 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
     <col min="5" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="24" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="24"/>
-    <col min="10" max="10" width="9.7109375" style="24" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="24" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.140625" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="24"/>
+    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="24"/>
+    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.109375" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -10192,7 +10297,7 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>317</v>
       </c>
@@ -10235,17 +10340,17 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
@@ -10255,7 +10360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -10263,24 +10368,24 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="24" customWidth="1"/>
     <col min="4" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
     <col min="7" max="7" width="15" style="24" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="24" customWidth="1"/>
     <col min="9" max="9" width="15" style="24" customWidth="1"/>
-    <col min="10" max="12" width="9.28515625" style="24" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="24" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="24"/>
+    <col min="10" max="12" width="9.33203125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -10327,7 +10432,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>334</v>
       </c>
@@ -10368,7 +10473,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>340</v>
       </c>
@@ -10414,7 +10519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -10422,20 +10527,20 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -10470,7 +10575,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>345</v>
       </c>
@@ -10518,7 +10623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE2"/>
   <sheetViews>
@@ -10526,14 +10631,14 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="75" max="75" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="75" max="75" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:135" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -10940,7 +11045,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:135" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -11323,7 +11428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE2"/>
   <sheetViews>
@@ -11331,15 +11436,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:135" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -11746,7 +11851,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:135" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>530</v>
       </c>
@@ -12128,7 +12233,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DA18"/>
   <sheetViews>
@@ -12136,82 +12255,82 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="23.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="23.5546875" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="14.42578125" customWidth="1"/>
-    <col min="29" max="29" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.5703125" customWidth="1"/>
-    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="21.85546875" customWidth="1"/>
-    <col min="60" max="60" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="15.85546875" customWidth="1"/>
-    <col min="62" max="62" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="17.5703125" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="14.44140625" customWidth="1"/>
+    <col min="29" max="29" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.5546875" customWidth="1"/>
+    <col min="34" max="34" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="21.88671875" customWidth="1"/>
+    <col min="60" max="60" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.88671875" customWidth="1"/>
+    <col min="62" max="62" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="17.5546875" customWidth="1"/>
     <col min="70" max="70" width="15" customWidth="1"/>
-    <col min="72" max="72" width="19.7109375" customWidth="1"/>
-    <col min="73" max="73" width="12.85546875" customWidth="1"/>
-    <col min="74" max="74" width="16.7109375" customWidth="1"/>
-    <col min="75" max="75" width="17.140625" customWidth="1"/>
-    <col min="76" max="76" width="12.85546875" customWidth="1"/>
-    <col min="77" max="77" width="15.85546875" customWidth="1"/>
-    <col min="78" max="78" width="14.140625" style="24" customWidth="1"/>
+    <col min="72" max="72" width="19.6640625" customWidth="1"/>
+    <col min="73" max="73" width="12.88671875" customWidth="1"/>
+    <col min="74" max="74" width="16.6640625" customWidth="1"/>
+    <col min="75" max="75" width="17.109375" customWidth="1"/>
+    <col min="76" max="76" width="12.88671875" customWidth="1"/>
+    <col min="77" max="77" width="15.88671875" customWidth="1"/>
+    <col min="78" max="78" width="14.109375" style="24" customWidth="1"/>
     <col min="79" max="79" width="15" style="24" customWidth="1"/>
-    <col min="80" max="80" width="19.28515625" style="24" customWidth="1"/>
+    <col min="80" max="80" width="19.33203125" style="24" customWidth="1"/>
     <col min="81" max="81" width="15" style="24" customWidth="1"/>
-    <col min="82" max="84" width="9.28515625" style="24" customWidth="1"/>
-    <col min="85" max="85" width="8.85546875" style="24" customWidth="1"/>
-    <col min="86" max="86" width="10.5703125" style="24" customWidth="1"/>
-    <col min="87" max="87" width="18.7109375" style="24" customWidth="1"/>
-    <col min="88" max="88" width="16.85546875" style="24" customWidth="1"/>
-    <col min="89" max="89" width="10.28515625" style="24" customWidth="1"/>
-    <col min="90" max="90" width="16.85546875" style="24" customWidth="1"/>
-    <col min="91" max="91" width="9.42578125" style="24" customWidth="1"/>
-    <col min="92" max="92" width="14.42578125" style="24" customWidth="1"/>
-    <col min="93" max="93" width="10.28515625" style="24" customWidth="1"/>
-    <col min="94" max="94" width="16.140625" style="24" customWidth="1"/>
-    <col min="95" max="95" width="17.7109375" style="24" customWidth="1"/>
-    <col min="97" max="97" width="11.7109375" customWidth="1"/>
-    <col min="98" max="105" width="17.7109375" style="24" customWidth="1"/>
+    <col min="82" max="84" width="9.33203125" style="24" customWidth="1"/>
+    <col min="85" max="85" width="8.88671875" style="24" customWidth="1"/>
+    <col min="86" max="86" width="10.5546875" style="24" customWidth="1"/>
+    <col min="87" max="87" width="18.6640625" style="24" customWidth="1"/>
+    <col min="88" max="88" width="16.88671875" style="24" customWidth="1"/>
+    <col min="89" max="89" width="10.33203125" style="24" customWidth="1"/>
+    <col min="90" max="90" width="16.88671875" style="24" customWidth="1"/>
+    <col min="91" max="91" width="9.44140625" style="24" customWidth="1"/>
+    <col min="92" max="92" width="14.44140625" style="24" customWidth="1"/>
+    <col min="93" max="93" width="10.33203125" style="24" customWidth="1"/>
+    <col min="94" max="94" width="16.109375" style="24" customWidth="1"/>
+    <col min="95" max="95" width="17.6640625" style="24" customWidth="1"/>
+    <col min="97" max="97" width="11.6640625" customWidth="1"/>
+    <col min="98" max="105" width="17.6640625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:105" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -12528,7 +12647,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="2" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -12821,7 +12940,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="3" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>545</v>
       </c>
@@ -13112,7 +13231,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="4" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>547</v>
       </c>
@@ -13403,7 +13522,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="5" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>549</v>
       </c>
@@ -13696,7 +13815,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="6" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>552</v>
       </c>
@@ -13989,7 +14108,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="7" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>554</v>
       </c>
@@ -14282,7 +14401,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="8" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>556</v>
       </c>
@@ -14577,7 +14696,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="9" spans="1:105" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:105" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>558</v>
       </c>
@@ -14868,7 +14987,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="10" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:105" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>560</v>
       </c>
@@ -15159,7 +15278,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="11" spans="1:105" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:105" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>562</v>
       </c>
@@ -15452,7 +15571,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="12" spans="1:105" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:105" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>723</v>
       </c>
@@ -15753,7 +15872,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="18" spans="82:82" x14ac:dyDescent="0.25">
+    <row r="18" spans="82:82" x14ac:dyDescent="0.3">
       <c r="CD18" s="24" t="s">
         <v>724</v>
       </c>
@@ -15792,7 +15911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK3"/>
   <sheetViews>
@@ -15800,20 +15919,20 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" customWidth="1"/>
     <col min="2" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" customWidth="1"/>
-    <col min="12" max="13" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" customWidth="1"/>
+    <col min="12" max="13" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -16004,7 +16123,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -16191,7 +16310,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -16372,7 +16491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FD177"/>
   <sheetViews>
@@ -16380,22 +16499,22 @@
       <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="93.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.42578125" customWidth="1"/>
-    <col min="66" max="66" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.5703125" customWidth="1"/>
-    <col min="97" max="97" width="10.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="93.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.44140625" customWidth="1"/>
+    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.5546875" customWidth="1"/>
+    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:160" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:160" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -16877,7 +16996,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="2" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -17329,7 +17448,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="3" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>140</v>
       </c>
@@ -17608,7 +17727,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:160" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:160" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>150</v>
       </c>
@@ -17887,7 +18006,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
@@ -18166,7 +18285,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>163</v>
       </c>
@@ -18445,7 +18564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>169</v>
       </c>
@@ -18726,7 +18845,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>175</v>
       </c>
@@ -19007,7 +19126,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:160" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:160" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>683</v>
       </c>
@@ -19421,7 +19540,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="10" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS10"/>
       <c r="CT10" t="s">
         <v>162</v>
@@ -19430,7 +19549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS11"/>
       <c r="CT11" t="s">
         <v>162</v>
@@ -19439,502 +19558,502 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS12"/>
     </row>
-    <row r="13" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:160" x14ac:dyDescent="0.3">
       <c r="CS16"/>
     </row>
-    <row r="17" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="17" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS17"/>
     </row>
-    <row r="18" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="18" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS18"/>
     </row>
-    <row r="19" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="19" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS19"/>
     </row>
-    <row r="20" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="20" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS20"/>
     </row>
-    <row r="21" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="21" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS21"/>
     </row>
-    <row r="22" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="22" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS22"/>
     </row>
-    <row r="23" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="23" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS23"/>
     </row>
-    <row r="24" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="24" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS24"/>
     </row>
-    <row r="25" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="25" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS25"/>
     </row>
-    <row r="26" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="26" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS26"/>
     </row>
-    <row r="27" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="27" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS27"/>
     </row>
-    <row r="28" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="28" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS28"/>
     </row>
-    <row r="29" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="29" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS29"/>
     </row>
-    <row r="30" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="30" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS30"/>
     </row>
-    <row r="31" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="31" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS31"/>
     </row>
-    <row r="32" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="32" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS32"/>
     </row>
-    <row r="33" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="33" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS33"/>
     </row>
-    <row r="34" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="34" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS34"/>
     </row>
-    <row r="35" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="35" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS35"/>
     </row>
-    <row r="36" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="36" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS36"/>
     </row>
-    <row r="37" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="37" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS37"/>
     </row>
-    <row r="38" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="38" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS38"/>
     </row>
-    <row r="39" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="39" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS39"/>
     </row>
-    <row r="40" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="40" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS40"/>
     </row>
-    <row r="41" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="41" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS41"/>
     </row>
-    <row r="42" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="42" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS42"/>
     </row>
-    <row r="43" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="43" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS43"/>
     </row>
-    <row r="44" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="44" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS44"/>
     </row>
-    <row r="45" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="45" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS45"/>
     </row>
-    <row r="46" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="46" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS46"/>
     </row>
-    <row r="47" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="47" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS47"/>
     </row>
-    <row r="48" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="48" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS48"/>
     </row>
-    <row r="49" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="49" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS49"/>
     </row>
-    <row r="50" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="50" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS50"/>
     </row>
-    <row r="51" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="51" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS51"/>
     </row>
-    <row r="52" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="52" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS52"/>
     </row>
-    <row r="53" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="53" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS53"/>
     </row>
-    <row r="54" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="54" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS54"/>
     </row>
-    <row r="55" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="55" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS55"/>
     </row>
-    <row r="56" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="56" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS56"/>
     </row>
-    <row r="57" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="57" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS57"/>
     </row>
-    <row r="58" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="58" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS58"/>
     </row>
-    <row r="59" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="59" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS59"/>
     </row>
-    <row r="60" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="60" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS60"/>
     </row>
-    <row r="61" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="61" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS61"/>
     </row>
-    <row r="62" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="62" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS62"/>
     </row>
-    <row r="63" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="63" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS63"/>
     </row>
-    <row r="64" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="64" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS64"/>
     </row>
-    <row r="65" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="65" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS65"/>
     </row>
-    <row r="66" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="66" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS66"/>
     </row>
-    <row r="67" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="67" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS67"/>
     </row>
-    <row r="68" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="68" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS68"/>
     </row>
-    <row r="69" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="69" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS69"/>
     </row>
-    <row r="70" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="70" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS70"/>
     </row>
-    <row r="71" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="71" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS71"/>
     </row>
-    <row r="72" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="72" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS72"/>
     </row>
-    <row r="73" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="73" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS73"/>
     </row>
-    <row r="74" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="74" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS74"/>
     </row>
-    <row r="75" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="75" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS75"/>
     </row>
-    <row r="76" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="76" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS76"/>
     </row>
-    <row r="77" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="77" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS77"/>
     </row>
-    <row r="78" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="78" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS78"/>
     </row>
-    <row r="79" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="79" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS79"/>
     </row>
-    <row r="80" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="80" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS80"/>
     </row>
-    <row r="81" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="81" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS81"/>
     </row>
-    <row r="82" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="82" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS82"/>
     </row>
-    <row r="83" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="83" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS83"/>
     </row>
-    <row r="84" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="84" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS84"/>
     </row>
-    <row r="85" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="85" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS85"/>
     </row>
-    <row r="86" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="86" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS86"/>
     </row>
-    <row r="87" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="87" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS87"/>
     </row>
-    <row r="88" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="88" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS88"/>
     </row>
-    <row r="89" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="89" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS89"/>
     </row>
-    <row r="90" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="90" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS90"/>
     </row>
-    <row r="91" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="91" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS91"/>
     </row>
-    <row r="92" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="92" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS92"/>
     </row>
-    <row r="93" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="93" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS93"/>
     </row>
-    <row r="94" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="94" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS94"/>
     </row>
-    <row r="95" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="95" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS95"/>
     </row>
-    <row r="96" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="96" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS96"/>
     </row>
-    <row r="97" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="97" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS97"/>
     </row>
-    <row r="98" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="98" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS98"/>
     </row>
-    <row r="99" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="99" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS99"/>
     </row>
-    <row r="100" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="100" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS100"/>
     </row>
-    <row r="101" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="101" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS101"/>
     </row>
-    <row r="102" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="102" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS102"/>
     </row>
-    <row r="103" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="103" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS103"/>
     </row>
-    <row r="104" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="104" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS104"/>
     </row>
-    <row r="105" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="105" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS105"/>
     </row>
-    <row r="106" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="106" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS106"/>
     </row>
-    <row r="107" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="107" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS107"/>
     </row>
-    <row r="108" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="108" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS108"/>
     </row>
-    <row r="109" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="109" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS109"/>
     </row>
-    <row r="110" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="110" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS110"/>
     </row>
-    <row r="111" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="111" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS111"/>
     </row>
-    <row r="112" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="112" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS112"/>
     </row>
-    <row r="113" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="113" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS113"/>
     </row>
-    <row r="114" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="114" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS114"/>
     </row>
-    <row r="115" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="115" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS115"/>
     </row>
-    <row r="116" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="116" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS116"/>
     </row>
-    <row r="117" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="117" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS117"/>
     </row>
-    <row r="118" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="118" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS118"/>
     </row>
-    <row r="119" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="119" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS119"/>
     </row>
-    <row r="120" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="120" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS120"/>
     </row>
-    <row r="121" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="121" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS121"/>
     </row>
-    <row r="122" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="122" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS122"/>
     </row>
-    <row r="123" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="123" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS123"/>
     </row>
-    <row r="124" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="124" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS124"/>
     </row>
-    <row r="125" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="125" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS125"/>
     </row>
-    <row r="126" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="126" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS126"/>
     </row>
-    <row r="127" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="127" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS127"/>
     </row>
-    <row r="128" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="128" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS128"/>
     </row>
-    <row r="129" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="129" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS129"/>
     </row>
-    <row r="130" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="130" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS130"/>
     </row>
-    <row r="131" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="131" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS131"/>
     </row>
-    <row r="132" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="132" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS132"/>
     </row>
-    <row r="133" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="133" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS133"/>
     </row>
-    <row r="134" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="134" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS134"/>
     </row>
-    <row r="135" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="135" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS135"/>
     </row>
-    <row r="136" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="136" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS136"/>
     </row>
-    <row r="137" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="137" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS137"/>
     </row>
-    <row r="138" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="138" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS138"/>
     </row>
-    <row r="139" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="139" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS139"/>
     </row>
-    <row r="140" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="140" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS140"/>
     </row>
-    <row r="141" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="141" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS141"/>
     </row>
-    <row r="142" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="142" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS142"/>
     </row>
-    <row r="143" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="143" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS143"/>
     </row>
-    <row r="144" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="144" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS144"/>
     </row>
-    <row r="145" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="145" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS145"/>
     </row>
-    <row r="146" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="146" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS146"/>
     </row>
-    <row r="147" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="147" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS147"/>
     </row>
-    <row r="148" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="148" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS148"/>
     </row>
-    <row r="149" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="149" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS149"/>
     </row>
-    <row r="150" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="150" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS150"/>
     </row>
-    <row r="151" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="151" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS151"/>
     </row>
-    <row r="152" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="152" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS152"/>
     </row>
-    <row r="153" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="153" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS153"/>
     </row>
-    <row r="154" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="154" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS154"/>
     </row>
-    <row r="155" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="155" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS155"/>
     </row>
-    <row r="156" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="156" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS156"/>
     </row>
-    <row r="157" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="157" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS157"/>
     </row>
-    <row r="158" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="158" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS158"/>
     </row>
-    <row r="159" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="159" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS159"/>
     </row>
-    <row r="160" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="160" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS160"/>
     </row>
-    <row r="161" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="161" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS161"/>
     </row>
-    <row r="162" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="162" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS162"/>
     </row>
-    <row r="163" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="163" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS163"/>
     </row>
-    <row r="164" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="164" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS164"/>
     </row>
-    <row r="165" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="165" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS165"/>
     </row>
-    <row r="166" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="166" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS166"/>
     </row>
-    <row r="167" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="167" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS167"/>
     </row>
-    <row r="168" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="168" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS168"/>
     </row>
-    <row r="169" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="169" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS169"/>
     </row>
-    <row r="170" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="170" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS170"/>
     </row>
-    <row r="171" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="171" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS171"/>
     </row>
-    <row r="172" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="172" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS172"/>
     </row>
-    <row r="173" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="173" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS173"/>
     </row>
-    <row r="174" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="174" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS174"/>
     </row>
-    <row r="175" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="175" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS175"/>
     </row>
-    <row r="176" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="176" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS176"/>
     </row>
-    <row r="177" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="177" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS177"/>
     </row>
   </sheetData>
@@ -19947,7 +20066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -19955,17 +20074,17 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -20000,7 +20119,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>186</v>
       </c>
@@ -20027,7 +20146,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>190</v>
       </c>
@@ -20058,7 +20177,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>191</v>
       </c>
@@ -20079,7 +20198,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>192</v>
       </c>
@@ -20107,7 +20226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -20115,14 +20234,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -20160,7 +20279,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>733</v>
       </c>
@@ -20206,7 +20325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
@@ -20214,19 +20333,19 @@
       <selection sqref="A1:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
     <col min="17" max="17" width="47" customWidth="1"/>
-    <col min="18" max="18" width="37.7109375" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -20277,7 +20396,7 @@
       </c>
       <c r="R1" s="20"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>201</v>
       </c>
@@ -20328,7 +20447,7 @@
       </c>
       <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>201</v>
       </c>
@@ -20379,7 +20498,7 @@
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>201</v>
       </c>
@@ -20430,7 +20549,7 @@
       </c>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>201</v>
       </c>
@@ -20481,7 +20600,7 @@
       </c>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>201</v>
       </c>
@@ -20537,7 +20656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -20545,13 +20664,13 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -20571,7 +20690,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>258</v>
       </c>
@@ -20591,7 +20710,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>262</v>
       </c>
@@ -20609,80 +20728,6 @@
       </c>
       <c r="F3" s="12" t="s">
         <v>261</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="G2" s="11">
-        <v>1888887</v>
-      </c>
-      <c r="H2" s="11">
-        <v>55554</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -20692,16 +20737,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -20709,84 +20754,54 @@
         <v>2</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>255</v>
+        <v>63</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>256</v>
+        <v>203</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>267</v>
+        <v>204</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="2">
-        <v>99</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="2">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" s="2">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
-        <v>271</v>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1888887</v>
+      </c>
+      <c r="H2" s="11">
+        <v>55554</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the missing header of Sheet10
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation2/TestData/TestData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4438" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="872">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2613,6 +2613,42 @@
   </si>
   <si>
     <t>TC_visaMoneyTransfer</t>
+  </si>
+  <si>
+    <t>DeviceTechnology</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>BranchID</t>
+  </si>
+  <si>
+    <t>CardPackID</t>
+  </si>
+  <si>
+    <t>DeviceNumber</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>CVV2</t>
+  </si>
+  <si>
+    <t>ICVV</t>
+  </si>
+  <si>
+    <t>PVKI</t>
+  </si>
+  <si>
+    <t>PinOffset</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>load</t>
   </si>
 </sst>
 </file>
@@ -2817,7 +2853,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2934,6 +2970,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -12235,14 +12273,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
+        <v>860</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>861</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>862</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>863</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>864</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>865</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>866</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>867</v>
+      </c>
+      <c r="I1" s="74" t="s">
+        <v>868</v>
+      </c>
+      <c r="J1" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="74" t="s">
+        <v>869</v>
+      </c>
+      <c r="L1" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="75" t="s">
+        <v>870</v>
+      </c>
+      <c r="N1" s="75" t="s">
+        <v>871</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>